<commit_message>
Adding STLs Updating BOM
</commit_message>
<xml_diff>
--- a/Hardware/DCZIA DC32 BADGE BOM.xlsx
+++ b/Hardware/DCZIA DC32 BADGE BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamster\Documents\Development\Personal\dczia\Defcon32-Badge\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamster\Documents\Development\Badges\dczia\Defcon32-Badge\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380C180E-55F1-46A9-AB40-F13123CBE661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150277AF-5675-435C-A385-F228CB140A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="180" windowWidth="27540" windowHeight="13596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1180" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -326,9 +326,6 @@
     <t>SW2</t>
   </si>
   <si>
-    <t>SC189ZULTRT</t>
-  </si>
-  <si>
     <t>3.3v regulator</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>62684-50210E9ALF</t>
   </si>
   <si>
-    <t>947-SC189ZULTRT</t>
-  </si>
-  <si>
     <t>Newark</t>
   </si>
   <si>
@@ -396,6 +390,12 @@
   </si>
   <si>
     <t>2520</t>
+  </si>
+  <si>
+    <t>947-SC189ZSKTRT</t>
+  </si>
+  <si>
+    <t>SC189ZSKTRT</t>
   </si>
 </sst>
 </file>
@@ -774,23 +774,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6328125" customWidth="1"/>
+    <col min="2" max="2" width="32.6328125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="6"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" style="6"/>
+    <col min="8" max="8" width="14.6328125" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -837,7 +837,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -856,14 +856,14 @@
       <c r="D4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>82</v>
       </c>
@@ -889,22 +889,22 @@
         <v>1</v>
       </c>
       <c r="J6" s="1">
-        <f>H6*I6</f>
+        <f t="shared" ref="J6:J20" si="0">H6*I6</f>
         <v>3.1E-2</v>
       </c>
       <c r="K6" s="1">
         <v>1000</v>
       </c>
       <c r="L6" s="1">
-        <f>IF((($N$2 * I6) - K6) &lt; 0, 0, (($N$2 * I6) - K6))</f>
+        <f t="shared" ref="L6:L21" si="1">IF((($N$2 * I6) - K6) &lt; 0, 0, (($N$2 * I6) - K6))</f>
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <f>L6*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M6:M20" si="2">L6*H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
@@ -912,13 +912,13 @@
         <v>25</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>42</v>
@@ -930,25 +930,25 @@
         <v>2</v>
       </c>
       <c r="J7" s="1">
-        <f>H7*I7</f>
+        <f t="shared" si="0"/>
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="1">
-        <f>IF((($N$2 * I7) - K7) &lt; 0, 0, (($N$2 * I7) - K7))</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="M7" s="1">
-        <f>L7*H7</f>
+        <f t="shared" si="2"/>
         <v>4.3999999999999995</v>
       </c>
       <c r="N7" s="1">
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>84</v>
       </c>
@@ -974,22 +974,22 @@
         <v>3</v>
       </c>
       <c r="J8" s="1">
-        <f>H8*I8</f>
+        <f t="shared" si="0"/>
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="K8" s="1">
         <v>1000</v>
       </c>
       <c r="L8" s="1">
-        <f>IF((($N$2 * I8) - K8) &lt; 0, 0, (($N$2 * I8) - K8))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M8" s="1">
-        <f>L8*H8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1010,22 +1010,22 @@
         <v>18</v>
       </c>
       <c r="J9" s="1">
-        <f>H9*I9</f>
+        <f t="shared" si="0"/>
         <v>0.42120000000000002</v>
       </c>
       <c r="K9" s="1">
         <v>3000</v>
       </c>
       <c r="L9" s="1">
-        <f>IF((($N$2 * I9) - K9) &lt; 0, 0, (($N$2 * I9) - K9))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M9" s="1">
-        <f>L9*H9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>85</v>
       </c>
@@ -1036,13 +1036,13 @@
         <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>87</v>
@@ -1054,25 +1054,25 @@
         <v>1</v>
       </c>
       <c r="J10" s="1">
-        <f>H10*I10</f>
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
       </c>
       <c r="L10" s="1">
-        <f>IF((($N$2 * I10) - K10) &lt; 0, 0, (($N$2 * I10) - K10))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M10" s="1">
-        <f>L10*H10</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N10" s="1">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
@@ -1093,22 +1093,22 @@
         <v>1</v>
       </c>
       <c r="J11" s="1">
-        <f>H11*I11</f>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="K11" s="1">
         <v>110</v>
       </c>
       <c r="L11" s="1">
-        <f>IF((($N$2 * I11) - K11) &lt; 0, 0, (($N$2 * I11) - K11))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <f>L11*H11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
@@ -1116,16 +1116,16 @@
         <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="1">
@@ -1135,25 +1135,25 @@
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <f>H12*I12</f>
+        <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
       </c>
       <c r="L12" s="1">
-        <f>IF((($N$2 * I12) - K12) &lt; 0, 0, (($N$2 * I12) - K12))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M12" s="1">
-        <f>L12*H12</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="N12" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1161,16 +1161,16 @@
         <v>91</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H13" s="1">
         <v>0.495</v>
@@ -1179,25 +1179,25 @@
         <v>1</v>
       </c>
       <c r="J13" s="1">
-        <f>H13*I13</f>
+        <f t="shared" si="0"/>
         <v>0.495</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <f>IF((($N$2 * I13) - K13) &lt; 0, 0, (($N$2 * I13) - K13))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M13" s="1">
-        <f>L13*H13</f>
+        <f t="shared" si="2"/>
         <v>49.5</v>
       </c>
       <c r="N13" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -1223,22 +1223,22 @@
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <f>H14*I14</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="K14" s="1">
         <v>5000</v>
       </c>
       <c r="L14" s="1">
-        <f>IF((($N$2 * I14) - K14) &lt; 0, 0, (($N$2 * I14) - K14))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <f>L14*H14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1264,22 +1264,22 @@
         <v>1</v>
       </c>
       <c r="J15" s="1">
-        <f>H15*I15</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="K15" s="1">
         <v>5000</v>
       </c>
       <c r="L15" s="1">
-        <f>IF((($N$2 * I15) - K15) &lt; 0, 0, (($N$2 * I15) - K15))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <f>L15*H15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>93</v>
       </c>
@@ -1305,22 +1305,22 @@
         <v>3</v>
       </c>
       <c r="J16" s="1">
-        <f>H16*I16</f>
+        <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="K16" s="1">
         <v>5000</v>
       </c>
       <c r="L16" s="1">
-        <f>IF((($N$2 * I16) - K16) &lt; 0, 0, (($N$2 * I16) - K16))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M16" s="1">
-        <f>L16*H16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>94</v>
       </c>
@@ -1346,22 +1346,22 @@
         <v>1</v>
       </c>
       <c r="J17" s="1">
-        <f>H17*I17</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="K17" s="1">
         <v>5000</v>
       </c>
       <c r="L17" s="1">
-        <f>IF((($N$2 * I17) - K17) &lt; 0, 0, (($N$2 * I17) - K17))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M17" s="1">
-        <f>L17*H17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>95</v>
       </c>
@@ -1385,25 +1385,25 @@
         <v>1</v>
       </c>
       <c r="J18" s="1">
-        <f>H18*I18</f>
+        <f t="shared" si="0"/>
         <v>0.50800000000000001</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
       </c>
       <c r="L18" s="1">
-        <f>IF((($N$2 * I18) - K18) &lt; 0, 0, (($N$2 * I18) - K18))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M18" s="1">
-        <f>L18*H18</f>
+        <f t="shared" si="2"/>
         <v>50.8</v>
       </c>
       <c r="N18" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>96</v>
       </c>
@@ -1427,39 +1427,39 @@
         <v>1</v>
       </c>
       <c r="J19" s="1">
-        <f>H19*I19</f>
+        <f t="shared" si="0"/>
         <v>0.98799999999999999</v>
       </c>
       <c r="K19" s="1">
         <v>0</v>
       </c>
       <c r="L19" s="1">
-        <f>IF((($N$2 * I19) - K19) &lt; 0, 0, (($N$2 * I19) - K19))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M19" s="1">
-        <f>L19*H19</f>
+        <f t="shared" si="2"/>
         <v>98.8</v>
       </c>
       <c r="N19" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="1">
@@ -1469,30 +1469,30 @@
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <f>H20*I20</f>
+        <f t="shared" si="0"/>
         <v>0.80400000000000005</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
       </c>
       <c r="L20" s="1">
-        <f>IF((($N$2 * I20) - K20) &lt; 0, 0, (($N$2 * I20) - K20))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M20" s="1">
-        <f>L20*H20</f>
+        <f t="shared" si="2"/>
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="G21" s="7"/>
       <c r="I21" s="1">
@@ -1502,11 +1502,11 @@
         <v>0</v>
       </c>
       <c r="L21" s="1">
-        <f>IF((($N$2 * I21) - K21) &lt; 0, 0, (($N$2 * I21) - K21))</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1533,25 +1533,25 @@
         <v>1</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" ref="J22:J37" si="0">H22*I22</f>
+        <f t="shared" ref="J22:J37" si="3">H22*I22</f>
         <v>6</v>
       </c>
       <c r="K22" s="1">
         <v>0</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" ref="L22:L37" si="1">IF((($N$2 * I22) - K22) &lt; 0, 0, (($N$2 * I22) - K22))</f>
+        <f t="shared" ref="L22:L37" si="4">IF((($N$2 * I22) - K22) &lt; 0, 0, (($N$2 * I22) - K22))</f>
         <v>100</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" ref="M22:M26" si="2">L22*H22</f>
+        <f t="shared" ref="M22:M26" si="5">L22*H22</f>
         <v>600</v>
       </c>
       <c r="N22" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="7"/>
@@ -1576,28 +1576,28 @@
         <v>1</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.69</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L24" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1615,30 +1615,30 @@
         <v>1</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.48</v>
       </c>
       <c r="K25" s="1">
         <v>110</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="1">
@@ -1648,52 +1648,52 @@
         <v>1</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.94</v>
       </c>
       <c r="K26" s="1">
         <v>0</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>794</v>
       </c>
       <c r="N26" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D27" s="7"/>
       <c r="G27" s="7"/>
       <c r="J27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="7"/>
       <c r="G28" s="7"/>
       <c r="J28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>50</v>
@@ -1710,18 +1710,18 @@
         <v>1</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K29" s="1">
         <v>0</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>51</v>
@@ -1738,18 +1738,18 @@
         <v>1</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="K30" s="1">
         <v>0</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>52</v>
@@ -1758,7 +1758,7 @@
         <v>69</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="1">
@@ -1768,18 +1768,18 @@
         <v>3</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.92999999999999994</v>
       </c>
       <c r="K31" s="1">
         <v>0</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>53</v>
@@ -1788,7 +1788,7 @@
         <v>69</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="1">
@@ -1798,21 +1798,21 @@
         <v>1</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.86</v>
       </c>
       <c r="K32" s="1">
         <v>0</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N32" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>54</v>
@@ -1821,7 +1821,7 @@
         <v>69</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="1">
@@ -1831,24 +1831,24 @@
         <v>1</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.186</v>
       </c>
       <c r="K33" s="1">
         <v>0</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N33" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>69</v>
@@ -1865,14 +1865,14 @@
         <v>125</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N34" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>56</v>
@@ -1883,18 +1883,18 @@
         <v>4</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K35" s="1">
         <v>0</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>57</v>
@@ -1905,41 +1905,41 @@
         <v>1</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K36" s="1">
         <v>0</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D37" s="7"/>
       <c r="G37" s="7"/>
       <c r="J37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="D38" s="8"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D39" s="7"/>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>71</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>27.786199999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>81</v>
       </c>
@@ -1969,938 +1969,938 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:14" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:14" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="12.5" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F17" r:id="rId1" display="https://www.mouser.com/ProductDetail/303-0603WAF1004T5E" xr:uid="{938DC35C-C5F4-43ED-B330-9F6C59021A94}"/>

</xml_diff>